<commit_message>
Add Web Scraping and Parsing the xPaths functionalities
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -446,34 +446,30 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>price</t>
+          <t>description</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>image</t>
+          <t>image_url</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.amazon.eg/%D8%AD%D8%B0%D8%A7%D8%A1-%D8%AA%D8%B2%D9%84%D8%AC-%D9%84%D9%84%D8%B1%D8%AC%D8%A7%D9%84-%D8%A7%D8%AF%D9%8A%D8%AF%D8%A7%D8%B3%D8%8C-%D8%A3%D8%B3%D9%88%D8%AF/dp/B0BPDWKP3B?ref=dlx_doubl_dg_dcl_B0BPDWKP3B_dt_sl7_ef</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Amazon Customer5.0 من 5 نجوم</t>
-        </is>
-      </c>
+          <t>https://www.jumia.com.eg/ar/catalog/?q=blouse</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>شميز حريمي أبيض ساده فورمال236.00 جنيه295.00 جنيه20%4.3 out of 5(167)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://m.media-amazon.com/images/G/42/personalization/ybh/loading-4x-gray._CB411329145_.gif</t>
+          <t>data:image/gif;base64,R0lGODlhAQABAIAAAAAAAP///yH5BAEAAAAALAAAAAABAAEAAAIBRAA7</t>
         </is>
       </c>
     </row>

</xml_diff>